<commit_message>
Multiline-Feature um Standard-Multiline-Kommandos erweitert implementiert
</commit_message>
<xml_diff>
--- a/examples-simple/src/test/resources/MultilineTest.xlsx
+++ b/examples-simple/src/test/resources/MultilineTest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ricvog01\IdeaProjects\jexunit\examples-simple\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B77E996E-65FB-471A-96B1-CE63F2429539}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF17948E-7F03-40EA-8F2B-94F30E235AA7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="48" windowWidth="21312" windowHeight="10032" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="27">
   <si>
     <t>false</t>
   </si>
@@ -89,6 +89,18 @@
   </si>
   <si>
     <t>multiLine</t>
+  </si>
+  <si>
+    <t>createPersonMultiline</t>
+  </si>
+  <si>
+    <t>Simon</t>
+  </si>
+  <si>
+    <t>Julian</t>
+  </si>
+  <si>
+    <t>Robert</t>
   </si>
 </sst>
 </file>
@@ -472,13 +484,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
@@ -645,7 +660,65 @@
         <v>10000</v>
       </c>
     </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="2">
+        <v>30266</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="2">
+        <v>41255</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" s="2">
+        <v>40544</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>